<commit_message>
血石系统 血石等级NumericType.Bloodstone 配置表PublicQiangHuaConfig 可以参考C2M_ItemQiangHuaRequest
</commit_message>
<xml_diff>
--- a/Excel/PublicQiangHuaConfig.xlsx
+++ b/Excel/PublicQiangHuaConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitWeiJing\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitWeiJing\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466AF7D9-B053-4D46-9302-759C05E987B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538D5EB-C299-42B5-BC87-DF62A0D8F5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipQiangHuaProto" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="M3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,579 +61,6 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">作者:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">10.生命值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">11.物理攻击       
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">14.魔法攻击
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">17.物理防御        
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">20.魔法防御
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">30.暴击
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">31.命中
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">32.闪避
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">33.物理免伤
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">34.魔法免伤
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">35.移动速度
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">36.伤害减免
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">50:血量百分比
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">51：物攻百分比
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">52：魔攻百分比
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">53：物防百分比
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">54：魔防百分比
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">101：格挡值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">111：重击概率
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">112:  重击附加伤害值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">121:  每次普通攻击附加的伤害值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">131:  忽视目标防御值   
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">132:  忽视目标魔防值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">133:  忽视目标百分比防御值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">134:  忽视目标百分比魔防值
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">141:  吸血概率
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">151:  法术反击
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">152:  攻击反击
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">161：韧性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">201：初始暴击等级
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">202：初始韧性等级
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">203：初始命中等级
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">204：初始闪避等级
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">301:光抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">302:暗抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">303:火抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">304:水抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">305:电抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">321：//野兽攻击抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">322：//人物攻击抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">323：//恶魔攻击抗性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">401：//经验加成
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">402：//金币加成
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">403：//洗炼极品掉落
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">404：//隐藏属性出现概率
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t>405：//装备上的宝石槽位出现概率</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">作者:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">属性类型，属性值     ;号间隔多个属性
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -1315,10 +742,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Id</t>
   </si>
@@ -1371,9 +795,6 @@
     <t>EquipPropreAdd</t>
   </si>
   <si>
-    <t>AddPropreListStr</t>
-  </si>
-  <si>
     <t>ItemSubType</t>
   </si>
   <si>
@@ -1488,6 +909,102 @@
   </si>
   <si>
     <t>强化类型</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_3</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_4</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_5</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_6</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_7</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>keji_8</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.01@220203;0.01</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.02@220203;0.02</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.03@220203;0.03</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.08@220203;0.08</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.1@220203;0.1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.12@220203;0.12</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.15@220203;0.15</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.175@220203;0.175</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.2@220203;0.2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.25@220203;0.25</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.3@220203;0.3</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>220103;0.35@220203;0.35</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1693,7 +1210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1721,6 +1238,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2881,19 +2401,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:IF18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="8.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16" style="3" customWidth="1"/>
-    <col min="6" max="10" width="14.125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="21.875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="24.875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16" style="3" customWidth="1"/>
+    <col min="4" max="5" width="14.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="11" width="14.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="21.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="24.875" style="3" customWidth="1"/>
     <col min="14" max="14" width="21.75" style="3" customWidth="1"/>
     <col min="15" max="240" width="8.875" style="3" customWidth="1"/>
   </cols>
@@ -2901,121 +2420,122 @@
     <row r="1" spans="3:240" s="1" customFormat="1" ht="14.25"/>
     <row r="2" spans="3:240" ht="13.5" customHeight="1">
       <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="3:240" ht="20.100000000000001" customHeight="1">
       <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="3:240" ht="20.100000000000001" customHeight="1">
       <c r="C4" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:240" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="3:240" ht="20.100000000000001" customHeight="1">
@@ -3023,31 +2543,31 @@
         <v>10100</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="12">
+        <v>48</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="8">
         <v>10101</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0</v>
       </c>
       <c r="H6" s="10">
         <v>0</v>
       </c>
       <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="J6" s="11">
+      <c r="K6" s="11">
         <v>30000</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
+      <c r="L6" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M6" s="10">
         <v>0</v>
@@ -3061,34 +2581,34 @@
         <v>10101</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="12">
+        <v>36</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>10102</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="10">
         <v>0</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <v>0.8</v>
       </c>
-      <c r="J7" s="11">
+      <c r="K7" s="11">
         <v>45000</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="M7" s="10">
-        <v>0</v>
+      <c r="L7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="N7" s="12">
         <v>0.05</v>
@@ -3099,34 +2619,34 @@
         <v>10102</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="12">
+        <v>37</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G8" s="8">
         <v>10103</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <v>0</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <v>0.7</v>
       </c>
-      <c r="J8" s="11">
+      <c r="K8" s="11">
         <v>60000</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0</v>
+      <c r="L8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="N8" s="12">
         <v>0.04</v>
@@ -3138,34 +2658,34 @@
         <v>10103</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="12">
+        <v>38</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="8">
         <v>10104</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>3</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="10">
         <v>5</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <v>0.6</v>
       </c>
-      <c r="J9" s="11">
+      <c r="K9" s="11">
         <v>75000</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="M9" s="10">
-        <v>0</v>
+      <c r="L9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="N9" s="12">
         <v>0.04</v>
@@ -3177,34 +2697,34 @@
         <v>10104</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="12">
+        <v>39</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="8">
         <v>10105</v>
       </c>
-      <c r="G10" s="10">
+      <c r="H10" s="10">
         <v>4</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>10</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <v>0.5</v>
       </c>
-      <c r="J10" s="11">
+      <c r="K10" s="11">
         <v>90000</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="M10" s="10">
-        <v>0</v>
+      <c r="L10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="N10" s="12">
         <v>0.03</v>
@@ -3216,34 +2736,34 @@
         <v>10105</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="12">
+        <v>40</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="8">
         <v>10106</v>
       </c>
-      <c r="G11" s="10">
+      <c r="H11" s="10">
         <v>5</v>
       </c>
-      <c r="H11" s="10">
+      <c r="I11" s="10">
         <v>15</v>
       </c>
-      <c r="I11" s="10">
+      <c r="J11" s="10">
         <v>0.4</v>
       </c>
-      <c r="J11" s="11">
+      <c r="K11" s="11">
         <v>120000</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="M11" s="10">
-        <v>0</v>
+      <c r="L11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="N11" s="12">
         <v>0.03</v>
@@ -3255,34 +2775,34 @@
         <v>10106</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="12">
+        <v>41</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="12">
         <v>1</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="8">
         <v>10107</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="10">
         <v>6</v>
       </c>
-      <c r="H12" s="10">
+      <c r="I12" s="10">
         <v>20</v>
       </c>
-      <c r="I12" s="10">
+      <c r="J12" s="10">
         <v>0.3</v>
       </c>
-      <c r="J12" s="11">
+      <c r="K12" s="11">
         <v>150000</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0.125</v>
-      </c>
-      <c r="M12" s="10">
-        <v>0</v>
+      <c r="L12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="N12" s="12">
         <v>0.02</v>
@@ -3294,34 +2814,34 @@
         <v>10107</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="12">
+        <v>42</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="12">
         <v>1</v>
       </c>
-      <c r="F13" s="8">
+      <c r="G13" s="8">
         <v>10108</v>
       </c>
-      <c r="G13" s="10">
+      <c r="H13" s="10">
         <v>7</v>
       </c>
-      <c r="H13" s="10">
+      <c r="I13" s="10">
         <v>25</v>
       </c>
-      <c r="I13" s="10">
+      <c r="J13" s="10">
         <v>0.25</v>
       </c>
-      <c r="J13" s="11">
+      <c r="K13" s="11">
         <v>180000</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0</v>
+      <c r="L13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="N13" s="12">
         <v>0.02</v>
@@ -3333,34 +2853,34 @@
         <v>10108</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="12">
+        <v>43</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="12">
         <v>1</v>
       </c>
-      <c r="F14" s="8">
+      <c r="G14" s="8">
         <v>10109</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="10">
         <v>8</v>
       </c>
-      <c r="H14" s="10">
+      <c r="I14" s="10">
         <v>30</v>
       </c>
-      <c r="I14" s="10">
+      <c r="J14" s="10">
         <v>0.2</v>
       </c>
-      <c r="J14" s="11">
+      <c r="K14" s="11">
         <v>240000</v>
       </c>
-      <c r="K14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
+      <c r="L14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="N14" s="12">
         <v>0.01</v>
@@ -3372,34 +2892,34 @@
         <v>10109</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="12">
+        <v>44</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="12">
         <v>1</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G15" s="8">
         <v>10110</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="10">
         <v>9</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I15" s="10">
         <v>35</v>
       </c>
-      <c r="I15" s="10">
+      <c r="J15" s="10">
         <v>0.1</v>
       </c>
-      <c r="J15" s="11">
+      <c r="K15" s="11">
         <v>300000</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="M15" s="10">
-        <v>0</v>
+      <c r="L15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="N15" s="12">
         <v>0.01</v>
@@ -3411,34 +2931,34 @@
         <v>10110</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="12">
+        <v>45</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="12">
         <v>1</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="8">
         <v>10111</v>
       </c>
-      <c r="G16" s="10">
+      <c r="H16" s="10">
         <v>10</v>
       </c>
-      <c r="H16" s="10">
+      <c r="I16" s="10">
         <v>40</v>
       </c>
-      <c r="I16" s="10">
+      <c r="J16" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>34</v>
-      </c>
       <c r="K16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="M16" s="10">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="N16" s="12">
         <v>5.0000000000000001E-3</v>
@@ -3450,34 +2970,34 @@
         <v>10111</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="12">
+        <v>46</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="8">
         <v>10112</v>
       </c>
-      <c r="G17" s="10">
+      <c r="H17" s="10">
         <v>11</v>
       </c>
-      <c r="H17" s="10">
+      <c r="I17" s="10">
         <v>45</v>
       </c>
-      <c r="I17" s="10">
+      <c r="J17" s="10">
         <v>0.05</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="K17" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="M17" s="10">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="N17" s="12">
         <v>5.0000000000000001E-3</v>
@@ -3489,34 +3009,34 @@
         <v>10112</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="12">
+        <v>47</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="12">
         <v>1</v>
       </c>
-      <c r="F18" s="10">
+      <c r="G18" s="10">
         <v>0</v>
       </c>
-      <c r="G18" s="10">
+      <c r="H18" s="10">
         <v>12</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I18" s="10">
         <v>50</v>
       </c>
-      <c r="I18" s="10">
+      <c r="J18" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="K18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="10">
-        <v>0.35</v>
-      </c>
-      <c r="M18" s="10">
-        <v>0</v>
+      <c r="M18" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="N18" s="12">
         <v>0.01</v>

</xml_diff>